<commit_message>
Adding data from Jan field work and associated script
</commit_message>
<xml_diff>
--- a/Data/benthic_interactions.xlsx
+++ b/Data/benthic_interactions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nina Bean\Documents\Projects\Benthic_interactions\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NinaBean/Documents/Documents - MacBook Air/Projects/Benthic_interactions/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060EA253-8684-4E34-890F-C77EFFD53FD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276DDEEB-D814-6146-ABC0-10B1DED4BCDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="0" windowWidth="18060" windowHeight="10130" xr2:uid="{4E0D5CF2-88E2-6D4C-A032-730E3D4667EB}"/>
+    <workbookView xWindow="220" yWindow="500" windowWidth="16860" windowHeight="17360" activeTab="2" xr2:uid="{4E0D5CF2-88E2-6D4C-A032-730E3D4667EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="3" r:id="rId1"/>
@@ -1652,7 +1652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C5CEC3-4086-4244-B3DD-3A1C141A5312}">
   <dimension ref="A1:AC352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="200" workbookViewId="0">
       <pane xSplit="9" ySplit="1" topLeftCell="K113" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
@@ -1660,18 +1660,18 @@
       <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.5" style="6" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="6.75" style="6" customWidth="1"/>
-    <col min="3" max="4" width="9.08203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="9" style="6" customWidth="1"/>
     <col min="5" max="5" width="4.83203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="9.08203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="2.58203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="9" style="6" customWidth="1"/>
+    <col min="7" max="7" width="2.5" style="6" customWidth="1"/>
     <col min="8" max="8" width="3.5" style="6" customWidth="1"/>
-    <col min="9" max="9" width="2.4140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="9.08203125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="5.25" style="6" customWidth="1"/>
+    <col min="9" max="9" width="2.33203125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="9" style="6" customWidth="1"/>
+    <col min="11" max="11" width="5.1640625" style="6" customWidth="1"/>
     <col min="12" max="12" width="7.33203125" style="6" customWidth="1"/>
     <col min="13" max="13" width="15.33203125" style="6" customWidth="1"/>
     <col min="14" max="21" width="7.33203125" style="6" customWidth="1"/>
@@ -1686,7 +1686,7 @@
     <col min="30" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>279</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>50</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>50</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="4" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>50</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="5" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>50</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="6" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>50</v>
       </c>
@@ -2226,7 +2226,7 @@
       </c>
       <c r="AC6" s="6"/>
     </row>
-    <row r="7" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>50</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="8" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>50</v>
       </c>
@@ -2396,7 +2396,7 @@
       <c r="AB8" s="6"/>
       <c r="AC8" s="6"/>
     </row>
-    <row r="9" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>50</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="10" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>50</v>
       </c>
@@ -2575,7 +2575,7 @@
       </c>
       <c r="AC10" s="6"/>
     </row>
-    <row r="11" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>50</v>
       </c>
@@ -2656,7 +2656,7 @@
       <c r="AB11" s="6"/>
       <c r="AC11" s="6"/>
     </row>
-    <row r="12" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>50</v>
       </c>
@@ -2737,7 +2737,7 @@
       <c r="AB12" s="6"/>
       <c r="AC12" s="6"/>
     </row>
-    <row r="13" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>50</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="14" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>50</v>
       </c>
@@ -2905,7 +2905,7 @@
       <c r="AB14" s="6"/>
       <c r="AC14" s="6"/>
     </row>
-    <row r="15" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="16" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>50</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="17" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>50</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="18" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>50</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="19" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>50</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="20" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>50</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="21" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>50</v>
       </c>
@@ -3504,7 +3504,7 @@
       <c r="AB21" s="6"/>
       <c r="AC21" s="6"/>
     </row>
-    <row r="22" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>50</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="23" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>50</v>
       </c>
@@ -3670,7 +3670,7 @@
       <c r="AB23" s="14"/>
       <c r="AC23" s="14"/>
     </row>
-    <row r="24" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>50</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="25" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>50</v>
       </c>
@@ -3838,7 +3838,7 @@
       <c r="AB25" s="6"/>
       <c r="AC25" s="6"/>
     </row>
-    <row r="26" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>50</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="27" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>50</v>
       </c>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="AC27" s="6"/>
     </row>
-    <row r="28" spans="1:29" s="5" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:29" s="5" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>50</v>
       </c>
@@ -4098,7 +4098,7 @@
       </c>
       <c r="AC28" s="6"/>
     </row>
-    <row r="29" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>50</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>50</v>
       </c>
@@ -4264,7 +4264,7 @@
       <c r="AB30" s="6"/>
       <c r="AC30" s="6"/>
     </row>
-    <row r="31" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>50</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="32" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>50</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="33" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>50</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="34" spans="1:29" s="5" customFormat="1" ht="23.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:29" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>50</v>
       </c>
@@ -4618,7 +4618,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="35" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>50</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="36" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>50</v>
       </c>
@@ -4792,7 +4792,7 @@
       </c>
       <c r="AC36" s="6"/>
     </row>
-    <row r="37" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>50</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="38" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>50</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="39" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>50</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>50</v>
       </c>
@@ -5132,7 +5132,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>50</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>50</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>50</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>50</v>
       </c>
@@ -5455,7 +5455,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>50</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>50</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>50</v>
       </c>
@@ -5704,7 +5704,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>50</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>50</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>50</v>
       </c>
@@ -5935,7 +5935,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>50</v>
       </c>
@@ -6021,7 +6021,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>50</v>
       </c>
@@ -6107,7 +6107,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>50</v>
       </c>
@@ -6198,7 +6198,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>50</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>50</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>46</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>50</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>50</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>50</v>
       </c>
@@ -6692,7 +6692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>50</v>
       </c>
@@ -6769,7 +6769,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>50</v>
       </c>
@@ -6847,7 +6847,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>50</v>
       </c>
@@ -6912,7 +6912,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>50</v>
       </c>
@@ -6983,7 +6983,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
         <v>50</v>
       </c>
@@ -7060,7 +7060,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
         <v>50</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>50</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
         <v>50</v>
       </c>
@@ -7294,7 +7294,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>50</v>
       </c>
@@ -7380,7 +7380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>50</v>
       </c>
@@ -7448,7 +7448,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
         <v>50</v>
       </c>
@@ -7516,7 +7516,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
         <v>50</v>
       </c>
@@ -7605,7 +7605,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>50</v>
       </c>
@@ -7682,7 +7682,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
         <v>50</v>
       </c>
@@ -7747,7 +7747,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
         <v>50</v>
       </c>
@@ -7836,7 +7836,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
         <v>50</v>
       </c>
@@ -7901,7 +7901,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
         <v>50</v>
       </c>
@@ -7978,7 +7978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
         <v>50</v>
       </c>
@@ -8043,7 +8043,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
         <v>46</v>
       </c>
@@ -8123,7 +8123,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
         <v>50</v>
       </c>
@@ -8191,7 +8191,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
         <v>50</v>
       </c>
@@ -8280,7 +8280,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
         <v>46</v>
       </c>
@@ -8357,7 +8357,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>50</v>
       </c>
@@ -8422,7 +8422,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>50</v>
       </c>
@@ -8496,7 +8496,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
         <v>50</v>
       </c>
@@ -8573,7 +8573,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
         <v>50</v>
       </c>
@@ -8650,7 +8650,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
         <v>50</v>
       </c>
@@ -8739,7 +8739,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
         <v>50</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
         <v>50</v>
       </c>
@@ -8884,7 +8884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
         <v>50</v>
       </c>
@@ -8949,7 +8949,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
         <v>50</v>
       </c>
@@ -9014,7 +9014,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
         <v>50</v>
       </c>
@@ -9091,7 +9091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
         <v>50</v>
       </c>
@@ -9165,7 +9165,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
         <v>50</v>
       </c>
@@ -9230,7 +9230,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="94" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
         <v>50</v>
       </c>
@@ -9307,7 +9307,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
         <v>46</v>
       </c>
@@ -9393,7 +9393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
         <v>50</v>
       </c>
@@ -9473,7 +9473,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
         <v>50</v>
       </c>
@@ -9555,7 +9555,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="98" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
         <v>50</v>
       </c>
@@ -9632,7 +9632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
         <v>50</v>
       </c>
@@ -9721,7 +9721,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
         <v>50</v>
       </c>
@@ -9789,7 +9789,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
         <v>50</v>
       </c>
@@ -9854,7 +9854,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
         <v>50</v>
       </c>
@@ -9943,7 +9943,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="103" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
         <v>50</v>
       </c>
@@ -10020,7 +10020,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
         <v>50</v>
       </c>
@@ -10094,7 +10094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
         <v>50</v>
       </c>
@@ -10159,7 +10159,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
         <v>50</v>
       </c>
@@ -10227,7 +10227,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
         <v>50</v>
       </c>
@@ -10292,7 +10292,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
         <v>50</v>
       </c>
@@ -10357,7 +10357,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A109" s="6" t="s">
         <v>50</v>
       </c>
@@ -10422,7 +10422,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
         <v>50</v>
       </c>
@@ -10496,7 +10496,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="111" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A111" s="6" t="s">
         <v>50</v>
       </c>
@@ -10573,7 +10573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A112" s="6" t="s">
         <v>50</v>
       </c>
@@ -10638,7 +10638,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="113" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
         <v>50</v>
       </c>
@@ -10703,7 +10703,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="114" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A114" s="6" t="s">
         <v>50</v>
       </c>
@@ -10768,7 +10768,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="115" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A115" s="6" t="s">
         <v>50</v>
       </c>
@@ -10833,7 +10833,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="116" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A116" s="6" t="s">
         <v>50</v>
       </c>
@@ -10898,7 +10898,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="117" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A117" s="6" t="s">
         <v>50</v>
       </c>
@@ -10957,7 +10957,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="118" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A118" s="6" t="s">
         <v>50</v>
       </c>
@@ -11022,7 +11022,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="119" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A119" s="6" t="s">
         <v>50</v>
       </c>
@@ -11087,7 +11087,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="120" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A120" s="6" t="s">
         <v>50</v>
       </c>
@@ -11149,7 +11149,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="121" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A121" s="6" t="s">
         <v>50</v>
       </c>
@@ -11208,7 +11208,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="122" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A122" s="6" t="s">
         <v>50</v>
       </c>
@@ -11267,7 +11267,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="123" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A123" s="6" t="s">
         <v>50</v>
       </c>
@@ -11329,7 +11329,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="124" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A124" s="6" t="s">
         <v>50</v>
       </c>
@@ -11388,7 +11388,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A125" s="6" t="s">
         <v>50</v>
       </c>
@@ -11453,7 +11453,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="126" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A126" s="6" t="s">
         <v>50</v>
       </c>
@@ -11518,7 +11518,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="127" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A127" s="6" t="s">
         <v>50</v>
       </c>
@@ -11586,7 +11586,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="128" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A128" s="6" t="s">
         <v>50</v>
       </c>
@@ -11654,7 +11654,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="129" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A129" s="6" t="s">
         <v>50</v>
       </c>
@@ -11722,7 +11722,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="130" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A130" s="6" t="s">
         <v>50</v>
       </c>
@@ -11790,7 +11790,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="131" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A131" s="6" t="s">
         <v>46</v>
       </c>
@@ -11855,7 +11855,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="132" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A132" s="6" t="s">
         <v>50</v>
       </c>
@@ -11917,7 +11917,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="133" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A133" s="6" t="s">
         <v>50</v>
       </c>
@@ -11979,7 +11979,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="134" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A134" s="6" t="s">
         <v>50</v>
       </c>
@@ -12041,7 +12041,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="135" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A135" s="6" t="s">
         <v>50</v>
       </c>
@@ -12106,7 +12106,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="136" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A136" s="6" t="s">
         <v>50</v>
       </c>
@@ -12165,7 +12165,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="137" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A137" s="6" t="s">
         <v>46</v>
       </c>
@@ -12233,7 +12233,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="138" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A138" s="6" t="s">
         <v>46</v>
       </c>
@@ -12298,7 +12298,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="139" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A139" s="6" t="s">
         <v>46</v>
       </c>
@@ -12363,7 +12363,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="140" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A140" s="6" t="s">
         <v>50</v>
       </c>
@@ -12422,7 +12422,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="141" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A141" s="6" t="s">
         <v>50</v>
       </c>
@@ -12493,7 +12493,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="142" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A142" s="6" t="s">
         <v>50</v>
       </c>
@@ -12561,7 +12561,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="143" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A143" s="6" t="s">
         <v>50</v>
       </c>
@@ -12620,7 +12620,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="144" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A144" s="6" t="s">
         <v>50</v>
       </c>
@@ -12685,7 +12685,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="145" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A145" s="6" t="s">
         <v>50</v>
       </c>
@@ -12750,7 +12750,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="146" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A146" s="6" t="s">
         <v>50</v>
       </c>
@@ -12821,7 +12821,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="147" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A147" s="6" t="s">
         <v>50</v>
       </c>
@@ -12883,7 +12883,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="148" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A148" s="6" t="s">
         <v>50</v>
       </c>
@@ -12945,7 +12945,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="149" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A149" s="6" t="s">
         <v>50</v>
       </c>
@@ -13013,7 +13013,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="150" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A150" s="6" t="s">
         <v>50</v>
       </c>
@@ -13081,7 +13081,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="151" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A151" s="6" t="s">
         <v>50</v>
       </c>
@@ -13140,7 +13140,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="152" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A152" s="6" t="s">
         <v>50</v>
       </c>
@@ -13205,7 +13205,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="153" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A153" s="6" t="s">
         <v>50</v>
       </c>
@@ -13267,7 +13267,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="154" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A154" s="6" t="s">
         <v>50</v>
       </c>
@@ -13329,7 +13329,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="155" spans="1:29" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:29" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="6" t="s">
         <v>50</v>
       </c>
@@ -13391,7 +13391,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="156" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A156" s="6" t="s">
         <v>50</v>
       </c>
@@ -13456,7 +13456,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="157" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A157" s="6" t="s">
         <v>50</v>
       </c>
@@ -13515,7 +13515,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="158" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A158" s="6" t="s">
         <v>50</v>
       </c>
@@ -13574,7 +13574,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="159" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A159" s="6" t="s">
         <v>50</v>
       </c>
@@ -13639,7 +13639,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="160" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A160" s="6" t="s">
         <v>50</v>
       </c>
@@ -13698,7 +13698,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="161" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A161" s="6" t="s">
         <v>50</v>
       </c>
@@ -13769,7 +13769,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="162" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A162" s="6" t="s">
         <v>50</v>
       </c>
@@ -13831,7 +13831,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="163" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A163" s="6" t="s">
         <v>50</v>
       </c>
@@ -13890,7 +13890,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="164" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A164" s="6" t="s">
         <v>50</v>
       </c>
@@ -13949,7 +13949,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="165" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A165" s="6" t="s">
         <v>50</v>
       </c>
@@ -14008,7 +14008,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="166" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A166" s="6" t="s">
         <v>50</v>
       </c>
@@ -14073,7 +14073,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="167" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A167" s="6" t="s">
         <v>46</v>
       </c>
@@ -14135,7 +14135,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="168" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A168" s="6" t="s">
         <v>46</v>
       </c>
@@ -14191,7 +14191,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="169" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A169" s="6" t="s">
         <v>50</v>
       </c>
@@ -14250,7 +14250,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="170" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A170" s="6" t="s">
         <v>50</v>
       </c>
@@ -14309,7 +14309,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="171" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A171" s="6" t="s">
         <v>50</v>
       </c>
@@ -14377,7 +14377,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="172" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A172" s="6" t="s">
         <v>50</v>
       </c>
@@ -14448,7 +14448,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="173" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A173" s="6" t="s">
         <v>50</v>
       </c>
@@ -14519,7 +14519,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="174" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A174" s="6" t="s">
         <v>50</v>
       </c>
@@ -14587,7 +14587,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="175" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A175" s="6" t="s">
         <v>50</v>
       </c>
@@ -14655,7 +14655,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="176" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A176" s="6" t="s">
         <v>50</v>
       </c>
@@ -14714,7 +14714,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="177" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A177" s="6" t="s">
         <v>50</v>
       </c>
@@ -14779,7 +14779,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="178" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A178" s="6" t="s">
         <v>50</v>
       </c>
@@ -14844,7 +14844,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="179" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A179" s="6" t="s">
         <v>50</v>
       </c>
@@ -14903,7 +14903,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="180" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A180" s="6" t="s">
         <v>50</v>
       </c>
@@ -14968,7 +14968,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="181" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A181" s="6" t="s">
         <v>50</v>
       </c>
@@ -15027,7 +15027,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="182" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A182" s="6" t="s">
         <v>50</v>
       </c>
@@ -15089,7 +15089,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="183" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A183" s="6" t="s">
         <v>50</v>
       </c>
@@ -15148,7 +15148,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="184" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A184" s="6" t="s">
         <v>50</v>
       </c>
@@ -15216,7 +15216,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="185" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A185" s="6" t="s">
         <v>50</v>
       </c>
@@ -15281,7 +15281,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="186" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A186" s="6" t="s">
         <v>50</v>
       </c>
@@ -15346,7 +15346,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="187" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A187" s="6" t="s">
         <v>50</v>
       </c>
@@ -15408,7 +15408,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="188" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A188" s="6" t="s">
         <v>50</v>
       </c>
@@ -15470,7 +15470,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="189" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A189" s="6" t="s">
         <v>50</v>
       </c>
@@ -15532,7 +15532,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="190" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A190" s="6" t="s">
         <v>50</v>
       </c>
@@ -15597,7 +15597,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="191" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A191" s="6" t="s">
         <v>50</v>
       </c>
@@ -15659,7 +15659,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="192" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A192" s="6" t="s">
         <v>50</v>
       </c>
@@ -15718,7 +15718,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="193" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A193" s="6" t="s">
         <v>50</v>
       </c>
@@ -15786,7 +15786,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="194" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A194" s="6" t="s">
         <v>50</v>
       </c>
@@ -15845,7 +15845,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="195" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A195" s="6" t="s">
         <v>50</v>
       </c>
@@ -15904,7 +15904,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="196" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A196" s="6" t="s">
         <v>50</v>
       </c>
@@ -15969,7 +15969,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="197" spans="1:29" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:29" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="6" t="s">
         <v>50</v>
       </c>
@@ -16034,7 +16034,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="198" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A198" s="6" t="s">
         <v>50</v>
       </c>
@@ -16105,7 +16105,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="199" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A199" s="6" t="s">
         <v>50</v>
       </c>
@@ -16176,7 +16176,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="200" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A200" s="6" t="s">
         <v>50</v>
       </c>
@@ -16241,7 +16241,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="201" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A201" s="6" t="s">
         <v>50</v>
       </c>
@@ -16300,7 +16300,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="202" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A202" s="6" t="s">
         <v>50</v>
       </c>
@@ -16359,7 +16359,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="203" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A203" s="6" t="s">
         <v>50</v>
       </c>
@@ -16418,7 +16418,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="204" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A204" s="6" t="s">
         <v>50</v>
       </c>
@@ -16477,7 +16477,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="205" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A205" s="6" t="s">
         <v>50</v>
       </c>
@@ -16536,7 +16536,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="206" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A206" s="6" t="s">
         <v>50</v>
       </c>
@@ -16595,7 +16595,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="207" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A207" s="6" t="s">
         <v>50</v>
       </c>
@@ -16654,7 +16654,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="208" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A208" s="6" t="s">
         <v>50</v>
       </c>
@@ -16713,7 +16713,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="209" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A209" s="6" t="s">
         <v>50</v>
       </c>
@@ -16772,7 +16772,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="210" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A210" s="6" t="s">
         <v>50</v>
       </c>
@@ -16831,7 +16831,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="211" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A211" s="6" t="s">
         <v>50</v>
       </c>
@@ -16896,7 +16896,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="212" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A212" s="6" t="s">
         <v>50</v>
       </c>
@@ -16964,7 +16964,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="213" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A213" s="6" t="s">
         <v>46</v>
       </c>
@@ -17026,7 +17026,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="214" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A214" s="6" t="s">
         <v>50</v>
       </c>
@@ -17085,7 +17085,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="215" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A215" s="6" t="s">
         <v>50</v>
       </c>
@@ -17144,7 +17144,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="216" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A216" s="6" t="s">
         <v>50</v>
       </c>
@@ -17203,7 +17203,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="217" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A217" s="6" t="s">
         <v>50</v>
       </c>
@@ -17268,7 +17268,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="218" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A218" s="6" t="s">
         <v>50</v>
       </c>
@@ -17336,7 +17336,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="219" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A219" s="6" t="s">
         <v>50</v>
       </c>
@@ -17404,7 +17404,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="220" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A220" s="6" t="s">
         <v>50</v>
       </c>
@@ -17469,7 +17469,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="221" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A221" s="6" t="s">
         <v>50</v>
       </c>
@@ -17528,7 +17528,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="222" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A222" s="6" t="s">
         <v>50</v>
       </c>
@@ -17587,7 +17587,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="223" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A223" s="6" t="s">
         <v>46</v>
       </c>
@@ -17643,7 +17643,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="224" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A224" s="6" t="s">
         <v>50</v>
       </c>
@@ -17705,7 +17705,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="225" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A225" s="6" t="s">
         <v>50</v>
       </c>
@@ -17764,7 +17764,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="226" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:29" ht="24" x14ac:dyDescent="0.3">
       <c r="A226" s="6" t="s">
         <v>50</v>
       </c>
@@ -17832,7 +17832,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="227" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A227" s="6" t="s">
         <v>50</v>
       </c>
@@ -17894,7 +17894,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="228" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A228" s="6" t="s">
         <v>50</v>
       </c>
@@ -17959,7 +17959,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="229" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A229" s="6" t="s">
         <v>50</v>
       </c>
@@ -18024,7 +18024,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="230" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A230" s="6" t="s">
         <v>50</v>
       </c>
@@ -18089,7 +18089,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="231" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A231" s="6" t="s">
         <v>50</v>
       </c>
@@ -18148,7 +18148,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="232" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A232" s="6" t="s">
         <v>50</v>
       </c>
@@ -18207,7 +18207,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="233" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A233" s="6" t="s">
         <v>50</v>
       </c>
@@ -18266,7 +18266,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="234" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A234" s="6" t="s">
         <v>50</v>
       </c>
@@ -18325,7 +18325,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="235" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A235" s="6" t="s">
         <v>50</v>
       </c>
@@ -18384,7 +18384,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="236" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A236" s="6" t="s">
         <v>50</v>
       </c>
@@ -18443,7 +18443,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="237" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A237" s="6" t="s">
         <v>50</v>
       </c>
@@ -18505,7 +18505,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="238" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A238" s="6" t="s">
         <v>50</v>
       </c>
@@ -18567,7 +18567,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="239" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A239" s="6" t="s">
         <v>46</v>
       </c>
@@ -18626,7 +18626,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="240" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A240" s="6" t="s">
         <v>46</v>
       </c>
@@ -18682,7 +18682,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="241" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A241" s="6" t="s">
         <v>50</v>
       </c>
@@ -18747,7 +18747,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="242" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A242" s="6" t="s">
         <v>50</v>
       </c>
@@ -18809,7 +18809,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="243" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A243" s="6" t="s">
         <v>50</v>
       </c>
@@ -18868,7 +18868,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="244" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A244" s="6" t="s">
         <v>50</v>
       </c>
@@ -18927,7 +18927,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="245" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A245" s="6" t="s">
         <v>50</v>
       </c>
@@ -18986,7 +18986,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="246" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A246" s="6" t="s">
         <v>50</v>
       </c>
@@ -19048,7 +19048,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="247" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A247" s="6" t="s">
         <v>50</v>
       </c>
@@ -19107,7 +19107,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="248" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A248" s="6" t="s">
         <v>50</v>
       </c>
@@ -19166,7 +19166,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="249" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A249" s="6" t="s">
         <v>50</v>
       </c>
@@ -19225,7 +19225,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="250" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A250" s="6" t="s">
         <v>50</v>
       </c>
@@ -19284,7 +19284,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="251" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A251" s="6" t="s">
         <v>50</v>
       </c>
@@ -19343,7 +19343,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="252" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A252" s="6" t="s">
         <v>50</v>
       </c>
@@ -19414,7 +19414,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="253" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A253" s="6" t="s">
         <v>50</v>
       </c>
@@ -19473,7 +19473,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="254" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A254" s="6" t="s">
         <v>50</v>
       </c>
@@ -19532,7 +19532,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="255" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A255" s="6" t="s">
         <v>50</v>
       </c>
@@ -19591,7 +19591,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="256" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A256" s="6" t="s">
         <v>50</v>
       </c>
@@ -19656,7 +19656,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="257" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A257" s="6" t="s">
         <v>50</v>
       </c>
@@ -19715,7 +19715,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="258" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A258" s="6" t="s">
         <v>50</v>
       </c>
@@ -19774,7 +19774,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="259" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A259" s="6" t="s">
         <v>50</v>
       </c>
@@ -19833,7 +19833,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="260" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A260" s="6" t="s">
         <v>50</v>
       </c>
@@ -19892,7 +19892,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="261" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A261" s="6" t="s">
         <v>50</v>
       </c>
@@ -19951,7 +19951,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="262" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A262" s="6" t="s">
         <v>50</v>
       </c>
@@ -20016,7 +20016,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="263" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A263" s="6" t="s">
         <v>50</v>
       </c>
@@ -20075,7 +20075,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="264" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A264" s="6" t="s">
         <v>50</v>
       </c>
@@ -20134,7 +20134,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="265" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A265" s="6" t="s">
         <v>50</v>
       </c>
@@ -20193,7 +20193,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="266" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A266" s="6" t="s">
         <v>50</v>
       </c>
@@ -20258,7 +20258,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="267" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A267" s="6" t="s">
         <v>50</v>
       </c>
@@ -20320,7 +20320,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="268" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A268" s="6" t="s">
         <v>50</v>
       </c>
@@ -20382,7 +20382,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="269" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A269" s="6" t="s">
         <v>50</v>
       </c>
@@ -20441,7 +20441,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="270" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A270" s="6" t="s">
         <v>50</v>
       </c>
@@ -20500,7 +20500,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="271" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A271" s="6" t="s">
         <v>50</v>
       </c>
@@ -20559,7 +20559,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="272" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A272" s="6" t="s">
         <v>50</v>
       </c>
@@ -20618,7 +20618,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="273" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A273" s="6" t="s">
         <v>50</v>
       </c>
@@ -20677,7 +20677,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="274" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A274" s="6" t="s">
         <v>50</v>
       </c>
@@ -20739,7 +20739,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="275" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A275" s="6" t="s">
         <v>50</v>
       </c>
@@ -20810,7 +20810,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="276" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A276" s="6" t="s">
         <v>50</v>
       </c>
@@ -20869,7 +20869,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="277" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A277" s="6" t="s">
         <v>50</v>
       </c>
@@ -20928,7 +20928,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="278" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A278" s="6" t="s">
         <v>50</v>
       </c>
@@ -20987,7 +20987,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="279" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A279" s="6" t="s">
         <v>50</v>
       </c>
@@ -21046,7 +21046,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="280" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A280" s="6" t="s">
         <v>50</v>
       </c>
@@ -21108,7 +21108,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="281" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A281" s="6" t="s">
         <v>50</v>
       </c>
@@ -21167,7 +21167,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="282" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A282" s="6" t="s">
         <v>46</v>
       </c>
@@ -21229,7 +21229,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="283" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A283" s="6" t="s">
         <v>46</v>
       </c>
@@ -21285,7 +21285,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="284" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A284" s="6" t="s">
         <v>50</v>
       </c>
@@ -21347,7 +21347,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="285" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A285" s="6" t="s">
         <v>50</v>
       </c>
@@ -21412,7 +21412,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="286" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A286" s="6" t="s">
         <v>50</v>
       </c>
@@ -21471,7 +21471,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="287" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A287" s="6" t="s">
         <v>50</v>
       </c>
@@ -21533,7 +21533,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="288" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A288" s="6" t="s">
         <v>50</v>
       </c>
@@ -21592,7 +21592,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="289" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A289" s="6" t="s">
         <v>50</v>
       </c>
@@ -21657,7 +21657,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="290" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A290" s="6" t="s">
         <v>50</v>
       </c>
@@ -21716,7 +21716,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="291" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A291" s="6" t="s">
         <v>50</v>
       </c>
@@ -21775,7 +21775,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="292" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A292" s="6" t="s">
         <v>50</v>
       </c>
@@ -21840,7 +21840,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="293" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A293" s="6" t="s">
         <v>50</v>
       </c>
@@ -21905,7 +21905,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="294" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A294" s="6" t="s">
         <v>50</v>
       </c>
@@ -21970,7 +21970,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="295" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A295" s="6" t="s">
         <v>50</v>
       </c>
@@ -22029,7 +22029,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="296" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A296" s="6" t="s">
         <v>50</v>
       </c>
@@ -22091,7 +22091,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="297" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A297" s="6" t="s">
         <v>50</v>
       </c>
@@ -22153,7 +22153,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="298" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A298" s="6" t="s">
         <v>50</v>
       </c>
@@ -22215,7 +22215,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="299" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A299" s="6" t="s">
         <v>50</v>
       </c>
@@ -22274,7 +22274,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="300" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A300" s="6" t="s">
         <v>50</v>
       </c>
@@ -22333,7 +22333,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="301" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A301" s="6" t="s">
         <v>46</v>
       </c>
@@ -22389,7 +22389,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="302" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A302" s="6" t="s">
         <v>46</v>
       </c>
@@ -22445,7 +22445,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="303" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A303" s="6" t="s">
         <v>46</v>
       </c>
@@ -22501,7 +22501,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="304" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A304" s="6" t="s">
         <v>46</v>
       </c>
@@ -22557,7 +22557,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="305" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A305" s="6" t="s">
         <v>46</v>
       </c>
@@ -22613,7 +22613,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="306" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A306" s="6" t="s">
         <v>46</v>
       </c>
@@ -22669,7 +22669,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="307" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A307" s="6" t="s">
         <v>46</v>
       </c>
@@ -22725,7 +22725,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="308" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A308" s="6" t="s">
         <v>46</v>
       </c>
@@ -22781,7 +22781,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="309" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A309" s="6" t="s">
         <v>46</v>
       </c>
@@ -22837,7 +22837,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="310" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A310" s="6" t="s">
         <v>46</v>
       </c>
@@ -22893,7 +22893,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="311" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A311" s="6" t="s">
         <v>46</v>
       </c>
@@ -22949,7 +22949,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="312" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A312" s="6" t="s">
         <v>46</v>
       </c>
@@ -23005,7 +23005,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="313" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A313" s="6" t="s">
         <v>46</v>
       </c>
@@ -23061,7 +23061,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="314" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A314" s="6" t="s">
         <v>46</v>
       </c>
@@ -23117,7 +23117,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="315" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A315" s="6" t="s">
         <v>46</v>
       </c>
@@ -23173,7 +23173,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="316" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A316" s="6" t="s">
         <v>46</v>
       </c>
@@ -23229,7 +23229,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="317" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A317" s="6" t="s">
         <v>46</v>
       </c>
@@ -23285,7 +23285,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="318" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A318" s="6" t="s">
         <v>46</v>
       </c>
@@ -23341,7 +23341,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="319" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A319" s="6" t="s">
         <v>46</v>
       </c>
@@ -23397,7 +23397,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="320" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A320" s="6" t="s">
         <v>46</v>
       </c>
@@ -23453,7 +23453,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="321" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A321" s="6" t="s">
         <v>46</v>
       </c>
@@ -23509,7 +23509,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="322" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A322" s="6" t="s">
         <v>46</v>
       </c>
@@ -23565,7 +23565,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="323" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A323" s="6" t="s">
         <v>46</v>
       </c>
@@ -23630,7 +23630,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="324" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A324" s="6" t="s">
         <v>46</v>
       </c>
@@ -23698,7 +23698,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="325" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A325" s="6" t="s">
         <v>46</v>
       </c>
@@ -23766,7 +23766,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="326" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A326" s="6" t="s">
         <v>46</v>
       </c>
@@ -23822,7 +23822,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="327" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A327" s="6" t="s">
         <v>50</v>
       </c>
@@ -23884,7 +23884,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="328" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A328" s="6" t="s">
         <v>50</v>
       </c>
@@ -23946,7 +23946,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="329" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A329" s="6" t="s">
         <v>50</v>
       </c>
@@ -24008,7 +24008,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="330" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A330" s="6" t="s">
         <v>50</v>
       </c>
@@ -24070,7 +24070,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="331" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A331" s="6" t="s">
         <v>50</v>
       </c>
@@ -24132,7 +24132,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="332" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A332" s="6" t="s">
         <v>50</v>
       </c>
@@ -24194,7 +24194,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="333" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A333" s="6" t="s">
         <v>50</v>
       </c>
@@ -24253,7 +24253,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="334" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A334" s="6" t="s">
         <v>50</v>
       </c>
@@ -24312,7 +24312,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="335" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A335" s="6" t="s">
         <v>50</v>
       </c>
@@ -24371,7 +24371,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="336" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A336" s="6" t="s">
         <v>50</v>
       </c>
@@ -24430,7 +24430,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="337" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A337" s="6" t="s">
         <v>50</v>
       </c>
@@ -24489,7 +24489,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="338" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A338" s="6" t="s">
         <v>50</v>
       </c>
@@ -24548,7 +24548,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="339" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A339" s="6" t="s">
         <v>50</v>
       </c>
@@ -24607,7 +24607,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="340" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A340" s="6" t="s">
         <v>50</v>
       </c>
@@ -24666,7 +24666,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="341" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A341" s="6" t="s">
         <v>50</v>
       </c>
@@ -24725,7 +24725,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="342" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A342" s="6" t="s">
         <v>46</v>
       </c>
@@ -24781,7 +24781,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="343" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A343" s="6" t="s">
         <v>46</v>
       </c>
@@ -24837,7 +24837,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="344" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A344" s="6" t="s">
         <v>46</v>
       </c>
@@ -24893,7 +24893,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="345" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A345" s="6" t="s">
         <v>46</v>
       </c>
@@ -24949,7 +24949,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="346" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A346" s="6" t="s">
         <v>46</v>
       </c>
@@ -25005,7 +25005,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="347" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A347" s="6" t="s">
         <v>46</v>
       </c>
@@ -25061,7 +25061,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="348" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A348" s="6" t="s">
         <v>46</v>
       </c>
@@ -25117,7 +25117,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="349" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A349" s="6" t="s">
         <v>46</v>
       </c>
@@ -25173,7 +25173,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="350" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A350" s="6" t="s">
         <v>46</v>
       </c>
@@ -25229,7 +25229,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="351" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A351" s="6" t="s">
         <v>46</v>
       </c>
@@ -25285,7 +25285,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="352" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A352" s="6" t="s">
         <v>46</v>
       </c>
@@ -25361,14 +25361,14 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.1640625" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="C1" s="24" t="s">
@@ -25376,7 +25376,7 @@
       </c>
       <c r="D1" s="24"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="10"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8" t="s">
@@ -25386,7 +25386,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>24</v>
       </c>
@@ -25404,7 +25404,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="23"/>
       <c r="B4" s="8" t="s">
         <v>302</v>
@@ -25420,7 +25420,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5">
         <f>SUM(C3:C4)</f>
         <v>70</v>
@@ -25434,7 +25434,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>304</v>
       </c>
@@ -25443,7 +25443,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -25452,7 +25452,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>305</v>
       </c>
@@ -25461,12 +25461,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>307</v>
       </c>
@@ -25485,16 +25485,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{376EDA95-0F2F-584D-B4EA-3BAA32E73A6E}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="63.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>108</v>
       </c>
@@ -25508,7 +25508,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>282</v>
       </c>
@@ -25519,7 +25519,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>284</v>
       </c>
@@ -25530,7 +25530,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>285</v>
       </c>
@@ -25538,7 +25538,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>291</v>
       </c>
@@ -25546,7 +25546,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>295</v>
       </c>
@@ -25557,7 +25557,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>296</v>
       </c>
@@ -25566,7 +25566,7 @@
       </c>
       <c r="D7" s="22"/>
     </row>
-    <row r="8" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>301</v>
       </c>
@@ -25575,7 +25575,7 @@
       </c>
       <c r="D8" s="22"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>345</v>
       </c>
@@ -25597,7 +25597,7 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" style="17" customWidth="1"/>
     <col min="2" max="2" width="8.1640625" style="17" bestFit="1" customWidth="1"/>
@@ -25616,7 +25616,7 @@
     <col min="15" max="16384" width="10.6640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>3</v>
       </c>
@@ -25639,7 +25639,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
@@ -25662,7 +25662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
@@ -25685,7 +25685,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>5</v>
       </c>
@@ -25699,7 +25699,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>5</v>
       </c>
@@ -25716,7 +25716,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>5</v>
       </c>
@@ -25727,7 +25727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>5</v>
       </c>
@@ -25738,7 +25738,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
@@ -25755,7 +25755,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>5</v>
       </c>
@@ -25772,7 +25772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>5</v>
       </c>
@@ -25783,7 +25783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>16</v>
       </c>
@@ -25800,7 +25800,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>16</v>
       </c>
@@ -25808,7 +25808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>16</v>
       </c>
@@ -25816,7 +25816,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>16</v>
       </c>
@@ -25827,7 +25827,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>16</v>
       </c>
@@ -25835,7 +25835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>16</v>
       </c>
@@ -25843,7 +25843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>16</v>
       </c>
@@ -25851,7 +25851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>16</v>
       </c>
@@ -25859,7 +25859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>16</v>
       </c>
@@ -25882,13 +25882,13 @@
       <selection pane="bottomLeft" activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="8.83203125" customWidth="1"/>
     <col min="9" max="9" width="55.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -25917,7 +25917,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -25943,7 +25943,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -25969,7 +25969,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -25992,7 +25992,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -26012,7 +26012,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -26032,7 +26032,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -26055,7 +26055,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -26078,7 +26078,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -26101,7 +26101,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -26124,7 +26124,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -26147,7 +26147,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -26170,7 +26170,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -26193,7 +26193,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -26216,7 +26216,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -26239,7 +26239,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -26262,7 +26262,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -26285,7 +26285,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -26308,7 +26308,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -26331,7 +26331,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -26354,7 +26354,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -26377,7 +26377,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -26397,7 +26397,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -26417,7 +26417,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -26440,7 +26440,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -26463,7 +26463,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -26486,7 +26486,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -26506,7 +26506,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -26526,7 +26526,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -26537,7 +26537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -26560,7 +26560,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -26580,7 +26580,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -26606,7 +26606,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -26626,7 +26626,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -26646,7 +26646,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -26666,7 +26666,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -26686,7 +26686,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -26706,7 +26706,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -26726,7 +26726,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -26746,7 +26746,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -26766,7 +26766,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -26786,7 +26786,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -26806,7 +26806,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -26826,7 +26826,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -26846,7 +26846,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -26866,7 +26866,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -26886,7 +26886,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -26906,7 +26906,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -26926,7 +26926,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -26946,7 +26946,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -26966,7 +26966,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -26986,7 +26986,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -27006,7 +27006,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -27026,7 +27026,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -27046,7 +27046,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -27063,7 +27063,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -27080,7 +27080,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>53</v>
       </c>
@@ -27097,7 +27097,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>53</v>
       </c>
@@ -27114,7 +27114,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>53</v>
       </c>
@@ -27131,7 +27131,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>53</v>
       </c>
@@ -27154,7 +27154,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>53</v>
       </c>
@@ -27177,7 +27177,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>53</v>
       </c>
@@ -27200,7 +27200,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>53</v>
       </c>
@@ -27223,7 +27223,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>53</v>
       </c>
@@ -27246,7 +27246,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>53</v>
       </c>
@@ -27269,7 +27269,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>53</v>
       </c>
@@ -27292,7 +27292,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>53</v>
       </c>
@@ -27318,7 +27318,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>53</v>
       </c>
@@ -27341,7 +27341,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>53</v>
       </c>
@@ -27358,7 +27358,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>53</v>
       </c>
@@ -27375,7 +27375,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>53</v>
       </c>
@@ -27398,7 +27398,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>53</v>
       </c>
@@ -27421,7 +27421,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>53</v>
       </c>
@@ -27444,7 +27444,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>53</v>
       </c>
@@ -27467,7 +27467,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>53</v>
       </c>
@@ -27490,7 +27490,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>53</v>
       </c>
@@ -27513,7 +27513,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>53</v>
       </c>
@@ -27536,7 +27536,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>53</v>
       </c>
@@ -27559,7 +27559,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>53</v>
       </c>
@@ -27582,7 +27582,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>53</v>
       </c>
@@ -27608,7 +27608,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>53</v>
       </c>
@@ -27634,7 +27634,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>53</v>
       </c>
@@ -27657,7 +27657,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>53</v>
       </c>
@@ -27680,7 +27680,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>53</v>
       </c>
@@ -27703,7 +27703,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>53</v>
       </c>
@@ -27726,7 +27726,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>53</v>
       </c>
@@ -27749,7 +27749,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>53</v>
       </c>
@@ -27772,7 +27772,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="91" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="6"/>
       <c r="B91" s="6" t="s">
         <v>46</v>
@@ -27823,7 +27823,7 @@
       <c r="Z91" s="6"/>
       <c r="AA91" s="6"/>
     </row>
-    <row r="92" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="6"/>
       <c r="B92" s="6" t="s">
         <v>46</v>
@@ -27872,7 +27872,7 @@
       <c r="Z92" s="6"/>
       <c r="AA92" s="6"/>
     </row>
-    <row r="93" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="6"/>
       <c r="B93" s="6" t="s">
         <v>46</v>
@@ -27923,7 +27923,7 @@
       <c r="Z93" s="6"/>
       <c r="AA93" s="6"/>
     </row>
-    <row r="94" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="6"/>
       <c r="B94" s="6" t="s">
         <v>46</v>
@@ -27972,7 +27972,7 @@
       <c r="Z94" s="6"/>
       <c r="AA94" s="6"/>
     </row>
-    <row r="95" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="6"/>
       <c r="B95" s="6" t="s">
         <v>46</v>
@@ -28021,7 +28021,7 @@
       <c r="Z95" s="6"/>
       <c r="AA95" s="6"/>
     </row>
-    <row r="96" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="6"/>
       <c r="B96" s="6" t="s">
         <v>46</v>
@@ -28070,7 +28070,7 @@
       <c r="Z96" s="6"/>
       <c r="AA96" s="6"/>
     </row>
-    <row r="97" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="6"/>
       <c r="B97" s="6" t="s">
         <v>46</v>
@@ -28119,7 +28119,7 @@
       <c r="Z97" s="6"/>
       <c r="AA97" s="6"/>
     </row>
-    <row r="98" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="6"/>
       <c r="B98" s="6" t="s">
         <v>46</v>
@@ -28168,7 +28168,7 @@
       <c r="Z98" s="6"/>
       <c r="AA98" s="6"/>
     </row>
-    <row r="99" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="6"/>
       <c r="B99" s="6" t="s">
         <v>46</v>
@@ -28217,7 +28217,7 @@
       <c r="Z99" s="6"/>
       <c r="AA99" s="6"/>
     </row>
-    <row r="100" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="6"/>
       <c r="B100" s="6" t="s">
         <v>46</v>
@@ -28266,7 +28266,7 @@
       <c r="Z100" s="6"/>
       <c r="AA100" s="6"/>
     </row>
-    <row r="101" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="6"/>
       <c r="B101" s="6" t="s">
         <v>46</v>
@@ -28315,7 +28315,7 @@
       <c r="Z101" s="6"/>
       <c r="AA101" s="6"/>
     </row>
-    <row r="102" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="6"/>
       <c r="B102" s="6" t="s">
         <v>46</v>
@@ -28364,7 +28364,7 @@
       <c r="Z102" s="6"/>
       <c r="AA102" s="6"/>
     </row>
-    <row r="103" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="6"/>
       <c r="B103" s="6" t="s">
         <v>46</v>
@@ -28415,7 +28415,7 @@
       <c r="Z103" s="6"/>
       <c r="AA103" s="6"/>
     </row>
-    <row r="104" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="6"/>
       <c r="B104" s="6" t="s">
         <v>46</v>
@@ -28466,7 +28466,7 @@
       <c r="Z104" s="6"/>
       <c r="AA104" s="6"/>
     </row>
-    <row r="105" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="6"/>
       <c r="B105" s="6" t="s">
         <v>46</v>
@@ -28515,7 +28515,7 @@
       <c r="Z105" s="6"/>
       <c r="AA105" s="6"/>
     </row>
-    <row r="106" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="6"/>
       <c r="B106" s="6" t="s">
         <v>46</v>
@@ -28580,12 +28580,12 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.5" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
@@ -28593,12 +28593,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>78</v>
       </c>
@@ -28606,12 +28606,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>74</v>
       </c>
@@ -28619,17 +28619,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>14</v>
       </c>
@@ -28640,27 +28640,27 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>10</v>
       </c>
@@ -28668,17 +28668,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
         <v>18</v>
       </c>
@@ -28686,7 +28686,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
         <v>85</v>
       </c>
@@ -28697,37 +28697,37 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
         <v>84</v>
       </c>

</xml_diff>